<commit_message>
Get all V1 api tests working
</commit_message>
<xml_diff>
--- a/molgenis-data-rest/src/test/resources/RestControllerV1_FileEMX.xlsx
+++ b/molgenis-data-rest/src/test/resources/RestControllerV1_FileEMX.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9980" yWindow="1220" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="9980" yWindow="1220" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="attributes" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>name</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t>file</t>
-  </si>
-  <si>
-    <t>fileAttr</t>
   </si>
   <si>
     <t>ApiTestFile</t>
@@ -95,17 +92,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -437,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -465,7 +466,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -476,10 +477,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -487,7 +488,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -500,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>